<commit_message>
Added computing the experience group
</commit_message>
<xml_diff>
--- a/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
+++ b/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ52"/>
+  <dimension ref="A1:CK52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,6 +661,11 @@
           <t>correctness</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>experience_group</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -983,6 +988,11 @@
       <c r="CJ2" t="n">
         <v>0.68</v>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1305,6 +1315,11 @@
       <c r="CJ3" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1626,6 +1641,11 @@
       </c>
       <c r="CJ4" t="n">
         <v>0.6</v>
+      </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -1949,6 +1969,11 @@
       <c r="CJ5" t="n">
         <v>0.82</v>
       </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2270,6 +2295,11 @@
       </c>
       <c r="CJ6" t="n">
         <v>0.9</v>
+      </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -2593,6 +2623,11 @@
       <c r="CJ7" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK7" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2915,6 +2950,11 @@
       <c r="CJ8" t="n">
         <v>0.96</v>
       </c>
+      <c r="CK8" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3237,6 +3277,11 @@
       <c r="CJ9" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK9" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3559,6 +3604,11 @@
       <c r="CJ10" t="n">
         <v>0.7</v>
       </c>
+      <c r="CK10" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3880,6 +3930,11 @@
       </c>
       <c r="CJ11" t="n">
         <v>0.8297872340425532</v>
+      </c>
+      <c r="CK11" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -4203,6 +4258,11 @@
       <c r="CJ12" t="n">
         <v>0.5102040816326531</v>
       </c>
+      <c r="CK12" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4525,6 +4585,11 @@
       <c r="CJ13" t="n">
         <v>0.9</v>
       </c>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>Network/IT admin</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4847,6 +4912,11 @@
       <c r="CJ14" t="n">
         <v>0.96</v>
       </c>
+      <c r="CK14" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -5169,6 +5239,11 @@
       <c r="CJ15" t="n">
         <v>0.76</v>
       </c>
+      <c r="CK15" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -5491,6 +5566,11 @@
       <c r="CJ16" t="n">
         <v>0.82</v>
       </c>
+      <c r="CK16" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -5813,6 +5893,11 @@
       <c r="CJ17" t="n">
         <v>0.5</v>
       </c>
+      <c r="CK17" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -6135,6 +6220,11 @@
       <c r="CJ18" t="n">
         <v>0.84</v>
       </c>
+      <c r="CK18" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -6457,6 +6547,11 @@
       <c r="CJ19" t="n">
         <v>0.7555555555555555</v>
       </c>
+      <c r="CK19" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -6778,6 +6873,11 @@
       </c>
       <c r="CJ20" t="n">
         <v>0.88</v>
+      </c>
+      <c r="CK20" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -7101,6 +7201,11 @@
       <c r="CJ21" t="n">
         <v>0.76</v>
       </c>
+      <c r="CK21" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -7423,6 +7528,11 @@
       <c r="CJ22" t="n">
         <v>0.58</v>
       </c>
+      <c r="CK22" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -7744,6 +7854,11 @@
       </c>
       <c r="CJ23" t="n">
         <v>0.88</v>
+      </c>
+      <c r="CK23" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -8067,6 +8182,11 @@
       <c r="CJ24" t="n">
         <v>0.88</v>
       </c>
+      <c r="CK24" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -8389,6 +8509,11 @@
       <c r="CJ25" t="n">
         <v>0.66</v>
       </c>
+      <c r="CK25" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -8711,6 +8836,11 @@
       <c r="CJ26" t="n">
         <v>0.6808510638297872</v>
       </c>
+      <c r="CK26" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -9033,6 +9163,11 @@
       <c r="CJ27" t="n">
         <v>0.9399999999999999</v>
       </c>
+      <c r="CK27" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -9355,6 +9490,11 @@
       <c r="CJ28" t="n">
         <v>0.72</v>
       </c>
+      <c r="CK28" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -9677,6 +9817,11 @@
       <c r="CJ29" t="n">
         <v>0.9591836734693877</v>
       </c>
+      <c r="CK29" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -9999,6 +10144,11 @@
       <c r="CJ30" t="n">
         <v>0.48</v>
       </c>
+      <c r="CK30" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -10321,6 +10471,11 @@
       <c r="CJ31" t="n">
         <v>0.98</v>
       </c>
+      <c r="CK31" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -10642,6 +10797,11 @@
       </c>
       <c r="CJ32" t="n">
         <v>0.851063829787234</v>
+      </c>
+      <c r="CK32" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -10965,6 +11125,11 @@
       <c r="CJ33" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK33" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -11287,6 +11452,11 @@
       <c r="CJ34" t="n">
         <v>0.5</v>
       </c>
+      <c r="CK34" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -11609,6 +11779,11 @@
       <c r="CJ35" t="n">
         <v>0.66</v>
       </c>
+      <c r="CK35" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -11931,6 +12106,11 @@
       <c r="CJ36" t="n">
         <v>0.8</v>
       </c>
+      <c r="CK36" t="inlineStr">
+        <is>
+          <t>Cyber security</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -12253,6 +12433,11 @@
       <c r="CJ37" t="n">
         <v>0.92</v>
       </c>
+      <c r="CK37" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -12574,6 +12759,11 @@
       </c>
       <c r="CJ38" t="n">
         <v>0.72</v>
+      </c>
+      <c r="CK38" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -12897,6 +13087,11 @@
       <c r="CJ39" t="n">
         <v>0.54</v>
       </c>
+      <c r="CK39" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -13219,6 +13414,11 @@
       <c r="CJ40" t="n">
         <v>0.54</v>
       </c>
+      <c r="CK40" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -13540,6 +13740,11 @@
       </c>
       <c r="CJ41" t="n">
         <v>0.5217391304347826</v>
+      </c>
+      <c r="CK41" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -13863,6 +14068,11 @@
       <c r="CJ42" t="n">
         <v>0.82</v>
       </c>
+      <c r="CK42" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -14185,6 +14395,11 @@
       <c r="CJ43" t="n">
         <v>0.84</v>
       </c>
+      <c r="CK43" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -14507,6 +14722,11 @@
       <c r="CJ44" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK44" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -14829,6 +15049,11 @@
       <c r="CJ45" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK45" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -15150,6 +15375,11 @@
       </c>
       <c r="CJ46" t="n">
         <v>0.84</v>
+      </c>
+      <c r="CK46" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -15473,6 +15703,11 @@
       <c r="CJ47" t="n">
         <v>0.96</v>
       </c>
+      <c r="CK47" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -15795,6 +16030,11 @@
       <c r="CJ48" t="n">
         <v>0.9</v>
       </c>
+      <c r="CK48" t="inlineStr">
+        <is>
+          <t>Cyber security</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -16117,6 +16357,11 @@
       <c r="CJ49" t="n">
         <v>0.74</v>
       </c>
+      <c r="CK49" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -16438,6 +16683,11 @@
       </c>
       <c r="CJ50" t="n">
         <v>0.8163265306122449</v>
+      </c>
+      <c r="CK50" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -16761,6 +17011,11 @@
       <c r="CJ51" t="n">
         <v>0.5208333333333334</v>
       </c>
+      <c r="CK51" t="inlineStr">
+        <is>
+          <t>Novice</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -17083,6 +17338,11 @@
       <c r="CJ52" t="n">
         <v>0.58</v>
       </c>
+      <c r="CK52" t="inlineStr">
+        <is>
+          <t>Novice+</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Experience group assignment and stats. Began work on calculating time to decide
</commit_message>
<xml_diff>
--- a/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
+++ b/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
@@ -4587,7 +4587,7 @@
       </c>
       <c r="CK13" t="inlineStr">
         <is>
-          <t>Network/IT admin</t>
+          <t>Practical</t>
         </is>
       </c>
     </row>
@@ -12108,7 +12108,7 @@
       </c>
       <c r="CK36" t="inlineStr">
         <is>
-          <t>Cyber security</t>
+          <t>Practical</t>
         </is>
       </c>
     </row>
@@ -16032,7 +16032,7 @@
       </c>
       <c r="CK48" t="inlineStr">
         <is>
-          <t>Cyber security</t>
+          <t>Practical</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Now keeping 25th in decision time. Commenting, additional analysis for HFES AM paper
</commit_message>
<xml_diff>
--- a/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
+++ b/excel/cry-wolf_20200125_14-35-09_patched_analysis.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -17345,6 +17412,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>